<commit_message>
updated nrmmol so that it doens't get called too many times. modified nmrproblem to deal with missing columns in excel sheets. Updated nmrproblem so that if excel worksheets are unticked they are not used in the calculation
</commit_message>
<xml_diff>
--- a/exampleProblems/Rotenone/Rotenone.xlsx
+++ b/exampleProblems/Rotenone/Rotenone.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ERIC\OneDrive - Durham University\projects\programming\2022\python\python\rdkit37\projects\simpleNMR\exampleProblems\Rotenone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/Rotenone/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_4EF8B8BE6A089523EB283CD275F1813C4B55408E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC4D98CA-57BB-449A-A1A8-F4EE037D2705}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="1005" windowWidth="20295" windowHeight="13620" activeTab="2"/>
+    <workbookView xWindow="3000" yWindow="1800" windowWidth="23880" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
@@ -33,8 +34,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="74">
   <si>
     <t>molecule</t>
   </si>
@@ -269,7 +268,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -394,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -426,6 +425,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +441,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -709,11 +705,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -748,7 +744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1292,554 +1288,554 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:J22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:13" ht="21">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5">
-      <c r="A2" s="11">
+    <row r="2" spans="1:13">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="1">
         <v>7.83</v>
       </c>
-      <c r="C2" s="11">
-        <v>129.93</v>
-      </c>
-      <c r="D2" s="11">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11">
+      <c r="C2" s="1">
+        <v>129.94999999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
         <v>16.59</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="1">
         <v>52.22</v>
       </c>
-      <c r="G2" s="11">
-        <v>0.35</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="G2" s="1">
+        <v>2.77</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="6"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="16.5">
-      <c r="A3" s="11">
+    <row r="3" spans="1:13">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="1">
         <v>6.76</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="1">
         <v>110.35</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="1">
         <v>0.1</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="1">
         <v>8.7799999999999994</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="1">
         <v>46.09</v>
       </c>
-      <c r="G3" s="11">
-        <v>0.31</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="G3" s="1">
+        <v>2.52</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="6"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="16.5">
-      <c r="A4" s="11">
+    <row r="4" spans="1:13">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="1">
         <v>6.49</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="1">
         <v>104.86</v>
       </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
         <v>16.649999999999999</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="1">
         <v>44.18</v>
       </c>
-      <c r="G4" s="11">
-        <v>0.31</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="G4" s="1">
+        <v>2.46</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="6"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="16.5">
-      <c r="A5" s="11">
+    <row r="5" spans="1:13">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="1">
         <v>6.44</v>
       </c>
-      <c r="C5" s="11">
-        <v>100.88</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="C5" s="1">
+        <v>100.89</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.1</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="1">
         <v>8.31</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="1">
         <v>42.58</v>
       </c>
-      <c r="G5" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
+      <c r="G5" s="1">
+        <v>2.42</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="6"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="16.5">
-      <c r="A6" s="11">
+    <row r="6" spans="1:13">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="1">
         <v>5.22</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="1">
         <v>87.81</v>
       </c>
-      <c r="D6" s="11">
-        <v>0</v>
-      </c>
-      <c r="E6" s="11">
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <v>22.3</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="1">
         <v>40.380000000000003</v>
       </c>
-      <c r="G6" s="11">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" spans="1:13" ht="16.5">
-      <c r="A7" s="11">
+      <c r="G6" s="1">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="1">
         <v>5.0599999999999996</v>
       </c>
-      <c r="C7" s="11">
-        <v>112.6</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="C7" s="1">
+        <v>112.53</v>
+      </c>
+      <c r="D7" s="1">
         <v>-1</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="1">
         <v>8.31</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="1">
         <v>55.12</v>
       </c>
-      <c r="G7" s="11">
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="G7" s="1">
+        <v>-2.2599999999999998</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="6"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="16.5">
-      <c r="A8" s="11">
+    <row r="8" spans="1:13">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="1">
         <v>4.92</v>
       </c>
-      <c r="C8" s="11">
-        <v>112.6</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C8" s="1">
+        <v>112.53</v>
+      </c>
+      <c r="D8" s="1">
         <v>-1</v>
       </c>
-      <c r="E8" s="11">
-        <v>11.81</v>
-      </c>
-      <c r="F8" s="11">
-        <v>15.01</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
+      <c r="E8" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="F8" s="1">
+        <v>54.72</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-2.4700000000000002</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="6"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="16.5">
-      <c r="A9" s="11">
+    <row r="9" spans="1:13">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="1">
         <v>4.91</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>72.2</v>
       </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="11">
-        <v>8.6</v>
-      </c>
-      <c r="F9" s="11">
-        <v>54.72</v>
-      </c>
-      <c r="G9" s="11">
-        <v>-0.31</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
+      <c r="D9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>11.58</v>
+      </c>
+      <c r="F9" s="1">
+        <v>39.11</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="6"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="16.5">
-      <c r="A10" s="11">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C10" s="11">
+      <c r="B10" s="1">
+        <v>4.59</v>
+      </c>
+      <c r="C10" s="1">
         <v>66.25</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="1">
         <v>-1</v>
       </c>
-      <c r="E10" s="11">
-        <v>12.16</v>
-      </c>
-      <c r="F10" s="11">
-        <v>10.83</v>
-      </c>
-      <c r="G10" s="11">
-        <v>-0.17</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="E10" s="1">
+        <v>12.02</v>
+      </c>
+      <c r="F10" s="1">
+        <v>57.22</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-0.67</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="6"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="16.5">
-      <c r="A11" s="11">
+    <row r="11" spans="1:13">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="1">
         <v>4.17</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="1">
         <v>66.25</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="1">
         <v>-1</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="1">
         <v>9.5500000000000007</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="1">
         <v>55.31</v>
       </c>
-      <c r="G11" s="11">
-        <v>-0.17</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+      <c r="G11" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="6"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="16.5">
-      <c r="A12" s="11">
+    <row r="12" spans="1:13">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="1">
         <v>3.83</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="1">
         <v>44.58</v>
       </c>
-      <c r="D12" s="11">
-        <v>0</v>
-      </c>
-      <c r="E12" s="11">
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
         <v>9.65</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="1">
         <v>56.83</v>
       </c>
-      <c r="G12" s="11">
-        <v>0.34</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-    </row>
-    <row r="13" spans="1:13" ht="16.5">
-      <c r="A13" s="11">
+      <c r="G12" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="1">
         <v>3.79</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="1">
         <v>55.83</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="1">
         <v>0.1</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="1">
         <v>11.17</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="1">
         <v>39.56</v>
       </c>
-      <c r="G13" s="11">
-        <v>0.72</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" ht="16.5">
-      <c r="A14" s="11">
+      <c r="G13" s="1">
+        <v>5.72</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="1">
         <v>3.75</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="1">
         <v>56.3</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="1">
         <v>0.1</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="1">
         <v>8.7200000000000006</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="1">
         <v>55.64</v>
       </c>
-      <c r="G14" s="11">
-        <v>0.74</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
+      <c r="G14" s="1">
+        <v>5.43</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="6"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="16.5">
-      <c r="A15" s="11">
+    <row r="15" spans="1:13">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="1">
         <v>3.3</v>
       </c>
-      <c r="C15" s="11">
-        <v>31.21</v>
-      </c>
-      <c r="D15" s="11">
+      <c r="C15" s="1">
+        <v>31.26</v>
+      </c>
+      <c r="D15" s="1">
         <v>-1</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="1">
         <v>10.42</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="1">
         <v>50.06</v>
       </c>
-      <c r="G15" s="11">
-        <v>-0.12</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+      <c r="G15" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="6"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:13" ht="16.5">
-      <c r="A16" s="11">
+    <row r="16" spans="1:13">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="1">
         <v>2.94</v>
       </c>
-      <c r="C16" s="11">
-        <v>31.21</v>
-      </c>
-      <c r="D16" s="11">
+      <c r="C16" s="1">
+        <v>31.26</v>
+      </c>
+      <c r="D16" s="1">
         <v>-1</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="1">
         <v>13.29</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="1">
         <v>48.98</v>
       </c>
-      <c r="G16" s="11">
-        <v>-0.13</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.5">
-      <c r="A17" s="11">
+      <c r="G16" s="1">
+        <v>-0.89</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="8">
         <v>1.75</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <v>17.11</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="8">
         <v>0.1</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="8">
         <v>9.64</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>39.950000000000003</v>
       </c>
-      <c r="G17" s="11">
-        <v>0.6</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+      <c r="G17" s="8">
+        <v>4.78</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" ht="16.5">
       <c r="A18" s="5"/>
@@ -1919,7 +1915,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3261,1771 +3257,799 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:A55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:11" ht="21">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5">
-      <c r="A2" s="11">
+    <row r="2" spans="1:11">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="1">
         <v>7.82</v>
       </c>
-      <c r="C2" s="11">
-        <v>157.88999999999999</v>
-      </c>
-      <c r="D2" s="11">
-        <v>87.3</v>
-      </c>
-      <c r="E2" s="11">
-        <v>5.31</v>
-      </c>
-      <c r="F2" s="11">
-        <v>52.84</v>
-      </c>
-      <c r="G2" s="11">
-        <v>4594.08</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" ht="16.5">
-      <c r="A3" s="11">
+      <c r="C2" s="1">
+        <v>188.9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>74.8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.98</v>
+      </c>
+      <c r="F2" s="1">
+        <v>19.23</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1606.65</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
-        <v>7.82</v>
-      </c>
-      <c r="C3" s="11">
-        <v>167.32</v>
-      </c>
-      <c r="D3" s="11">
-        <v>27.9</v>
-      </c>
-      <c r="E3" s="11">
-        <v>5.41</v>
-      </c>
-      <c r="F3" s="11">
-        <v>51.11</v>
-      </c>
-      <c r="G3" s="11">
-        <v>1445.74</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="1:11" ht="16.5">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11">
-        <v>7.82</v>
-      </c>
-      <c r="C4" s="11">
-        <v>188.88</v>
-      </c>
-      <c r="D4" s="11">
-        <v>44</v>
-      </c>
-      <c r="E4" s="11">
-        <v>4.47</v>
-      </c>
-      <c r="F4" s="11">
-        <v>52.17</v>
-      </c>
-      <c r="G4" s="11">
-        <v>1923.61</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" spans="1:11" ht="16.5">
-      <c r="A5" s="11">
+      <c r="B3" s="1">
+        <v>6.49</v>
+      </c>
+      <c r="C3" s="1">
+        <v>113.31</v>
+      </c>
+      <c r="D3" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.98</v>
+      </c>
+      <c r="F3" s="1">
+        <v>68.989999999999995</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1323.8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="11">
-        <v>6.77</v>
-      </c>
-      <c r="C5" s="11">
-        <v>147.35</v>
-      </c>
-      <c r="D5" s="11">
-        <v>95</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="B4" s="1">
+        <v>5.22</v>
+      </c>
+      <c r="C4" s="1">
+        <v>17.11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7.44</v>
+      </c>
+      <c r="F4" s="1">
+        <v>55.91</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2015.93</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
         <v>5.0599999999999996</v>
       </c>
-      <c r="F5" s="11">
-        <v>52.05</v>
-      </c>
-      <c r="G5" s="11">
-        <v>4696.4799999999996</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.5">
-      <c r="A6" s="11">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11">
-        <v>6.77</v>
-      </c>
-      <c r="C6" s="11">
-        <v>149.46</v>
-      </c>
-      <c r="D6" s="11">
-        <v>97.8</v>
-      </c>
-      <c r="E6" s="11">
-        <v>5.03</v>
-      </c>
-      <c r="F6" s="11">
-        <v>51.62</v>
-      </c>
-      <c r="G6" s="11">
-        <v>4770.71</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" spans="1:11" ht="16.5">
-      <c r="A7" s="11">
+      <c r="C5" s="1">
+        <v>17.11</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
+        <v>7.74</v>
+      </c>
+      <c r="F5" s="1">
+        <v>53.81</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1569.06</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" s="12" customFormat="1">
+      <c r="A6" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
-        <v>6.76</v>
-      </c>
-      <c r="C7" s="11">
-        <v>44.02</v>
-      </c>
-      <c r="D7" s="11">
-        <v>3.6</v>
-      </c>
-      <c r="E7" s="11">
-        <v>3.48</v>
-      </c>
-      <c r="F7" s="11">
-        <v>26.02</v>
-      </c>
-      <c r="G7" s="11">
-        <v>61.18</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5">
-      <c r="A8" s="11">
+      <c r="B6" s="1">
+        <v>4.92</v>
+      </c>
+      <c r="C6" s="1">
+        <v>17.11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>13.81</v>
+      </c>
+      <c r="F6" s="1">
+        <v>56.61</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5881.68</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="12" customFormat="1">
+      <c r="A7" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="11">
-        <v>6.76</v>
-      </c>
-      <c r="C8" s="11">
-        <v>104.81</v>
-      </c>
-      <c r="D8" s="11">
-        <v>47.2</v>
-      </c>
-      <c r="E8" s="11">
-        <v>7.49</v>
-      </c>
-      <c r="F8" s="11">
-        <v>52.32</v>
-      </c>
-      <c r="G8" s="11">
-        <v>3465.64</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5">
-      <c r="A9" s="11">
+      <c r="B7" s="1">
+        <v>4.59</v>
+      </c>
+      <c r="C7" s="1">
+        <v>147.34</v>
+      </c>
+      <c r="D7" s="1">
+        <v>117</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.98</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5.63</v>
+      </c>
+      <c r="G7" s="1">
+        <v>736.79</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="12" customFormat="1">
+      <c r="A8" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="11">
-        <v>6.75</v>
-      </c>
-      <c r="C9" s="11">
-        <v>143.83000000000001</v>
-      </c>
-      <c r="D9" s="11">
-        <v>73.900000000000006</v>
-      </c>
-      <c r="E9" s="11">
-        <v>9.3699999999999992</v>
-      </c>
-      <c r="F9" s="11">
-        <v>52.56</v>
-      </c>
-      <c r="G9" s="11">
-        <v>6823.43</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-    </row>
-    <row r="10" spans="1:11" ht="16.5">
-      <c r="A10" s="11">
+      <c r="B8" s="1">
+        <v>3.79</v>
+      </c>
+      <c r="C8" s="1">
+        <v>149.47</v>
+      </c>
+      <c r="D8" s="1">
+        <v>372.3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4.46</v>
+      </c>
+      <c r="F8" s="1">
+        <v>10.44</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6511.38</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="12" customFormat="1">
+      <c r="A9" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
-        <v>6.5</v>
-      </c>
-      <c r="C10" s="11">
-        <v>167.32</v>
-      </c>
-      <c r="D10" s="11">
-        <v>39.4</v>
-      </c>
-      <c r="E10" s="11">
-        <v>5.7</v>
-      </c>
-      <c r="F10" s="11">
-        <v>51.68</v>
-      </c>
-      <c r="G10" s="11">
-        <v>2175.52</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" ht="16.5">
-      <c r="A11" s="11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11">
-        <v>6.49</v>
-      </c>
-      <c r="C11" s="11">
-        <v>113.31</v>
-      </c>
-      <c r="D11" s="11">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="E11" s="11">
-        <v>4.47</v>
-      </c>
-      <c r="F11" s="11">
-        <v>48.28</v>
-      </c>
-      <c r="G11" s="11">
-        <v>1406.1</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="1:11" ht="16.5">
-      <c r="A12" s="11">
-        <v>11</v>
-      </c>
-      <c r="B12" s="11">
-        <v>6.49</v>
-      </c>
-      <c r="C12" s="11">
-        <v>157.88999999999999</v>
-      </c>
-      <c r="D12" s="11">
-        <v>23</v>
-      </c>
-      <c r="E12" s="11">
-        <v>5.5</v>
-      </c>
-      <c r="F12" s="11">
-        <v>51.36</v>
-      </c>
-      <c r="G12" s="11">
-        <v>1215.57</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-    </row>
-    <row r="13" spans="1:11" ht="16.5">
-      <c r="A13" s="11">
-        <v>12</v>
-      </c>
-      <c r="B13" s="11">
-        <v>6.44</v>
-      </c>
-      <c r="C13" s="11">
-        <v>104.81</v>
-      </c>
-      <c r="D13" s="11">
-        <v>123.3</v>
-      </c>
-      <c r="E13" s="11">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="F13" s="11">
-        <v>52.4</v>
-      </c>
-      <c r="G13" s="11">
-        <v>5324.22</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-    </row>
-    <row r="14" spans="1:11" ht="16.5">
-      <c r="A14" s="11">
-        <v>13</v>
-      </c>
-      <c r="B14" s="11">
-        <v>6.44</v>
-      </c>
-      <c r="C14" s="11">
-        <v>147.35</v>
-      </c>
-      <c r="D14" s="11">
-        <v>111.1</v>
-      </c>
-      <c r="E14" s="11">
-        <v>4.21</v>
-      </c>
-      <c r="F14" s="11">
-        <v>51.53</v>
-      </c>
-      <c r="G14" s="11">
-        <v>4518.55</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.5">
-      <c r="A15" s="11">
-        <v>14</v>
-      </c>
-      <c r="B15" s="11">
-        <v>6.44</v>
-      </c>
-      <c r="C15" s="11">
-        <v>44.59</v>
-      </c>
-      <c r="D15" s="11">
-        <v>30.6</v>
-      </c>
-      <c r="E15" s="11">
-        <v>5.73</v>
-      </c>
-      <c r="F15" s="11">
-        <v>52.18</v>
-      </c>
-      <c r="G15" s="11">
-        <v>1717.52</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-    </row>
-    <row r="16" spans="1:11" ht="16.5">
-      <c r="A16" s="11">
-        <v>15</v>
-      </c>
-      <c r="B16" s="11">
-        <v>6.43</v>
-      </c>
-      <c r="C16" s="11">
-        <v>149.46</v>
-      </c>
-      <c r="D16" s="11">
-        <v>101.9</v>
-      </c>
-      <c r="E16" s="11">
-        <v>4.72</v>
-      </c>
-      <c r="F16" s="11">
-        <v>50.92</v>
-      </c>
-      <c r="G16" s="11">
-        <v>4590.3</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-    </row>
-    <row r="17" spans="1:22" ht="16.5">
-      <c r="A17" s="11">
-        <v>16</v>
-      </c>
-      <c r="B17" s="11">
-        <v>6.43</v>
-      </c>
-      <c r="C17" s="11">
-        <v>143.83000000000001</v>
-      </c>
-      <c r="D17" s="11">
-        <v>138</v>
-      </c>
-      <c r="E17" s="11">
-        <v>4.78</v>
-      </c>
-      <c r="F17" s="11">
-        <v>51.75</v>
-      </c>
-      <c r="G17" s="11">
-        <v>6403.28</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-    </row>
-    <row r="18" spans="1:22" ht="16.5">
-      <c r="A18" s="11">
-        <v>17</v>
-      </c>
-      <c r="B18" s="11">
-        <v>5.22</v>
-      </c>
-      <c r="C18" s="11">
-        <v>31.31</v>
-      </c>
-      <c r="D18" s="11">
-        <v>4.8</v>
-      </c>
-      <c r="E18" s="11">
-        <v>2.98</v>
-      </c>
-      <c r="F18" s="11">
-        <v>53.43</v>
-      </c>
-      <c r="G18" s="11">
-        <v>141.87</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-    </row>
-    <row r="19" spans="1:22" ht="16.5">
-      <c r="A19" s="11">
-        <f>A18+1</f>
-        <v>18</v>
-      </c>
-      <c r="B19" s="11">
-        <v>5.0599999999999996</v>
-      </c>
-      <c r="C19" s="11">
-        <v>87.82</v>
-      </c>
-      <c r="D19" s="11">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="E19" s="11">
-        <v>10.14</v>
-      </c>
-      <c r="F19" s="11">
-        <v>53.64</v>
-      </c>
-      <c r="G19" s="11">
-        <v>3908.12</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-    </row>
-    <row r="20" spans="1:22" ht="16.5">
-      <c r="A20" s="11">
-        <f t="shared" ref="A20:A55" si="0">A19+1</f>
-        <v>19</v>
-      </c>
-      <c r="B20" s="11">
-        <v>5.0599999999999996</v>
-      </c>
-      <c r="C20" s="11">
-        <v>143.01</v>
-      </c>
-      <c r="D20" s="11">
-        <v>18.2</v>
-      </c>
-      <c r="E20" s="11">
-        <v>9.49</v>
-      </c>
-      <c r="F20" s="11">
-        <v>54.44</v>
-      </c>
-      <c r="G20" s="11">
-        <v>1765.63</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-    </row>
-    <row r="21" spans="1:22" ht="16.5">
-      <c r="A21" s="11">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="11">
-        <v>5.05</v>
-      </c>
-      <c r="C21" s="11">
-        <v>17.11</v>
-      </c>
-      <c r="D21" s="11">
-        <v>27.8</v>
-      </c>
-      <c r="E21" s="11">
-        <v>8.44</v>
-      </c>
-      <c r="F21" s="11">
-        <v>54.04</v>
-      </c>
-      <c r="G21" s="11">
-        <v>2380.9899999999998</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+      <c r="B9" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="C9" s="1">
+        <v>143.86000000000001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>376.1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4.18</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10.59</v>
+      </c>
+      <c r="G9" s="1">
+        <v>6249.99</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="J10" s="1"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="J11" s="1"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="J12" s="1"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="J13" s="1"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="J14" s="1"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="J15" s="1"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="J16" s="1"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="J17" s="1"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="J18" s="1"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="J19" s="1"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="J20" s="1"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:22" ht="16.5">
-      <c r="A22" s="11">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="11">
-        <v>4.92</v>
-      </c>
-      <c r="C22" s="11">
-        <v>17.11</v>
-      </c>
-      <c r="D22" s="11">
-        <v>20.9</v>
-      </c>
-      <c r="E22" s="11">
-        <v>13.81</v>
-      </c>
-      <c r="F22" s="11">
-        <v>56.6</v>
-      </c>
-      <c r="G22" s="11">
-        <v>3065.35</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:22" ht="16.5">
-      <c r="A23" s="11">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="11">
-        <v>4.91</v>
-      </c>
-      <c r="C23" s="11">
-        <v>104.81</v>
-      </c>
-      <c r="D23" s="11">
-        <v>36.5</v>
-      </c>
-      <c r="E23" s="11">
-        <v>7.8</v>
-      </c>
-      <c r="F23" s="11">
-        <v>52.83</v>
-      </c>
-      <c r="G23" s="11">
-        <v>2825.44</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
       <c r="J23" s="11"/>
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:22" ht="16.5">
-      <c r="A24" s="11">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="11">
-        <v>4.91</v>
-      </c>
-      <c r="C24" s="11">
-        <v>188.88</v>
-      </c>
-      <c r="D24" s="11">
-        <v>19.2</v>
-      </c>
-      <c r="E24" s="11">
-        <v>9.81</v>
-      </c>
-      <c r="F24" s="11">
-        <v>52.17</v>
-      </c>
-      <c r="G24" s="11">
-        <v>1840.03</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J24" s="11"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="10"/>
       <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:22" ht="16.5">
-      <c r="A25" s="11">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="11">
-        <v>4.59</v>
-      </c>
-      <c r="C25" s="11">
-        <v>188.88</v>
-      </c>
-      <c r="D25" s="11">
-        <v>46.2</v>
-      </c>
-      <c r="E25" s="11">
-        <v>18.63</v>
-      </c>
-      <c r="F25" s="11">
-        <v>51.61</v>
-      </c>
-      <c r="G25" s="11">
-        <v>8329.25</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
       <c r="J25" s="10"/>
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:22" ht="16.5">
-      <c r="A26" s="11">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="11">
-        <v>4.59</v>
-      </c>
-      <c r="C26" s="11">
-        <v>44.59</v>
-      </c>
-      <c r="D26" s="11">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="E26" s="11">
-        <v>25.79</v>
-      </c>
-      <c r="F26" s="11">
-        <v>51.36</v>
-      </c>
-      <c r="G26" s="11">
-        <v>17736.009999999998</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
       <c r="J26" s="10"/>
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:22" ht="16.5">
-      <c r="A27" s="11">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="11">
-        <v>4.59</v>
-      </c>
-      <c r="C27" s="11">
-        <v>72.180000000000007</v>
-      </c>
-      <c r="D27" s="11">
-        <v>55.3</v>
-      </c>
-      <c r="E27" s="11">
-        <v>24.5</v>
-      </c>
-      <c r="F27" s="11">
-        <v>52.28</v>
-      </c>
-      <c r="G27" s="11">
-        <v>13295.32</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
       <c r="J27" s="10"/>
       <c r="K27" s="11"/>
     </row>
     <row r="28" spans="1:22" ht="16.5">
-      <c r="A28" s="11">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="11">
-        <v>4.59</v>
-      </c>
-      <c r="C28" s="11">
-        <v>147.35</v>
-      </c>
-      <c r="D28" s="11">
-        <v>62.1</v>
-      </c>
-      <c r="E28" s="11">
-        <v>21.17</v>
-      </c>
-      <c r="F28" s="11">
-        <v>52.03</v>
-      </c>
-      <c r="G28" s="11">
-        <v>12837.98</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
       <c r="J28" s="10"/>
       <c r="K28" s="11"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
     </row>
     <row r="29" spans="1:22" ht="16.5">
-      <c r="A29" s="11">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="11">
-        <v>4.17</v>
-      </c>
-      <c r="C29" s="11">
-        <v>44.59</v>
-      </c>
-      <c r="D29" s="11">
-        <v>20.6</v>
-      </c>
-      <c r="E29" s="11">
-        <v>18.3</v>
-      </c>
-      <c r="F29" s="11">
-        <v>55.58</v>
-      </c>
-      <c r="G29" s="11">
-        <v>3929.08</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
       <c r="J29" s="10"/>
       <c r="K29" s="11"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12"/>
-      <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
-      <c r="U29" s="12"/>
-      <c r="V29" s="12"/>
     </row>
     <row r="30" spans="1:22" ht="16.5">
-      <c r="A30" s="11">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="11">
-        <v>4.17</v>
-      </c>
-      <c r="C30" s="11">
-        <v>157.88999999999999</v>
-      </c>
-      <c r="D30" s="11">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="E30" s="11">
-        <v>18.84</v>
-      </c>
-      <c r="F30" s="11">
-        <v>53.91</v>
-      </c>
-      <c r="G30" s="11">
-        <v>3215.84</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
       <c r="J30" s="10"/>
       <c r="K30" s="11"/>
     </row>
     <row r="31" spans="1:22" ht="16.5">
-      <c r="A31" s="11">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="11">
-        <v>4.16</v>
-      </c>
-      <c r="C31" s="11">
-        <v>72.180000000000007</v>
-      </c>
-      <c r="D31" s="11">
-        <v>46.4</v>
-      </c>
-      <c r="E31" s="11">
-        <v>19.02</v>
-      </c>
-      <c r="F31" s="11">
-        <v>52.9</v>
-      </c>
-      <c r="G31" s="11">
-        <v>8754.33</v>
-      </c>
-      <c r="H31" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
       <c r="J31" s="10"/>
       <c r="K31" s="11"/>
     </row>
     <row r="32" spans="1:22" ht="16.5">
-      <c r="A32" s="11">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="11">
-        <v>3.83</v>
-      </c>
-      <c r="C32" s="11">
-        <v>104.81</v>
-      </c>
-      <c r="D32" s="11">
-        <v>64.2</v>
-      </c>
-      <c r="E32" s="11">
-        <v>17.28</v>
-      </c>
-      <c r="F32" s="11">
-        <v>52.63</v>
-      </c>
-      <c r="G32" s="11">
-        <v>10949.03</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
       <c r="J32" s="10"/>
       <c r="K32" s="11"/>
     </row>
     <row r="33" spans="1:11" ht="16.5">
-      <c r="A33" s="11">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="11">
-        <v>3.83</v>
-      </c>
-      <c r="C33" s="11">
-        <v>113.31</v>
-      </c>
-      <c r="D33" s="11">
-        <v>18.3</v>
-      </c>
-      <c r="E33" s="11">
-        <v>8.2799999999999994</v>
-      </c>
-      <c r="F33" s="11">
-        <v>52.46</v>
-      </c>
-      <c r="G33" s="11">
-        <v>1491.77</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
       <c r="J33" s="10"/>
       <c r="K33" s="11"/>
     </row>
     <row r="34" spans="1:11" ht="16.5">
-      <c r="A34" s="11">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" s="11">
-        <v>3.83</v>
-      </c>
-      <c r="C34" s="11">
-        <v>100.89</v>
-      </c>
-      <c r="D34" s="11">
-        <v>22.5</v>
-      </c>
-      <c r="E34" s="11">
-        <v>7.83</v>
-      </c>
-      <c r="F34" s="11">
-        <v>55.21</v>
-      </c>
-      <c r="G34" s="11">
-        <v>1824.03</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
       <c r="J34" s="10"/>
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="1:11" ht="16.5">
-      <c r="A35" s="11">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B35" s="11">
-        <v>3.83</v>
-      </c>
-      <c r="C35" s="11">
-        <v>147.35</v>
-      </c>
-      <c r="D35" s="11">
-        <v>61.3</v>
-      </c>
-      <c r="E35" s="11">
-        <v>8.6</v>
-      </c>
-      <c r="F35" s="11">
-        <v>52.07</v>
-      </c>
-      <c r="G35" s="11">
-        <v>5148.0600000000004</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
       <c r="J35" s="10"/>
       <c r="K35" s="11"/>
     </row>
     <row r="36" spans="1:11" ht="16.5">
-      <c r="A36" s="11">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B36" s="11">
-        <v>3.83</v>
-      </c>
-      <c r="C36" s="11">
-        <v>143.83000000000001</v>
-      </c>
-      <c r="D36" s="11">
-        <v>25.2</v>
-      </c>
-      <c r="E36" s="11">
-        <v>8.69</v>
-      </c>
-      <c r="F36" s="11">
-        <v>51.98</v>
-      </c>
-      <c r="G36" s="11">
-        <v>2136.3200000000002</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
       <c r="J36" s="10"/>
       <c r="K36" s="11"/>
     </row>
     <row r="37" spans="1:11" ht="16.5">
-      <c r="A37" s="11">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B37" s="11">
-        <v>3.83</v>
-      </c>
-      <c r="C37" s="11">
-        <v>149.46</v>
-      </c>
-      <c r="D37" s="11">
-        <v>22.9</v>
-      </c>
-      <c r="E37" s="11">
-        <v>8.61</v>
-      </c>
-      <c r="F37" s="11">
-        <v>52.71</v>
-      </c>
-      <c r="G37" s="11">
-        <v>1952.56</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
       <c r="J37" s="10"/>
       <c r="K37" s="11"/>
     </row>
     <row r="38" spans="1:11" ht="16.5">
-      <c r="A38" s="11">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B38" s="11">
-        <v>3.83</v>
-      </c>
-      <c r="C38" s="11">
-        <v>110.32</v>
-      </c>
-      <c r="D38" s="11">
-        <v>36.1</v>
-      </c>
-      <c r="E38" s="11">
-        <v>8.69</v>
-      </c>
-      <c r="F38" s="11">
-        <v>52.82</v>
-      </c>
-      <c r="G38" s="11">
-        <v>3111.93</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
       <c r="J38" s="10"/>
       <c r="K38" s="11"/>
     </row>
     <row r="39" spans="1:11" ht="16.5">
-      <c r="A39" s="11">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B39" s="11">
-        <v>3.82</v>
-      </c>
-      <c r="C39" s="11">
-        <v>188.88</v>
-      </c>
-      <c r="D39" s="11">
-        <v>62.9</v>
-      </c>
-      <c r="E39" s="11">
-        <v>7.58</v>
-      </c>
-      <c r="F39" s="11">
-        <v>51.78</v>
-      </c>
-      <c r="G39" s="11">
-        <v>4629</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
       <c r="J39" s="10"/>
       <c r="K39" s="11"/>
     </row>
     <row r="40" spans="1:11" ht="16.5">
-      <c r="A40" s="11">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B40" s="11">
-        <v>3.79</v>
-      </c>
-      <c r="C40" s="11">
-        <v>149.16</v>
-      </c>
-      <c r="D40" s="11">
-        <v>3.5</v>
-      </c>
-      <c r="E40" s="11">
-        <v>4.7</v>
-      </c>
-      <c r="F40" s="11">
-        <v>10.94</v>
-      </c>
-      <c r="G40" s="11">
-        <v>33.520000000000003</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J40" s="10"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
       <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:11" ht="16.5">
-      <c r="A41" s="11">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B41" s="11">
-        <v>3.75</v>
-      </c>
-      <c r="C41" s="11">
-        <v>143.82</v>
-      </c>
-      <c r="D41" s="11">
-        <v>114.6</v>
-      </c>
-      <c r="E41" s="11">
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="F41" s="11">
-        <v>51.63</v>
-      </c>
-      <c r="G41" s="11">
-        <v>4844.7299999999996</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
     </row>
     <row r="42" spans="1:11" ht="16.5">
-      <c r="A42" s="11">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C42" s="11">
-        <v>143.01</v>
-      </c>
-      <c r="D42" s="11">
-        <v>36.1</v>
-      </c>
-      <c r="E42" s="11">
-        <v>32.99</v>
-      </c>
-      <c r="F42" s="11">
-        <v>55.92</v>
-      </c>
-      <c r="G42" s="11">
-        <v>12480.95</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
     </row>
     <row r="43" spans="1:11" ht="16.5">
-      <c r="A43" s="11">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C43" s="11">
-        <v>167.32</v>
-      </c>
-      <c r="D43" s="11">
-        <v>34.9</v>
-      </c>
-      <c r="E43" s="11">
-        <v>32.67</v>
-      </c>
-      <c r="F43" s="11">
-        <v>55</v>
-      </c>
-      <c r="G43" s="11">
-        <v>11779.25</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
     </row>
     <row r="44" spans="1:11" ht="16.5">
-      <c r="A44" s="11">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C44" s="11">
-        <v>87.82</v>
-      </c>
-      <c r="D44" s="11">
-        <v>15.9</v>
-      </c>
-      <c r="E44" s="11">
-        <v>31.25</v>
-      </c>
-      <c r="F44" s="11">
-        <v>56.48</v>
-      </c>
-      <c r="G44" s="11">
-        <v>5271.1</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I44" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
     </row>
     <row r="45" spans="1:11" ht="16.5">
-      <c r="A45" s="11">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C45" s="11">
-        <v>157.88999999999999</v>
-      </c>
-      <c r="D45" s="11">
-        <v>22.7</v>
-      </c>
-      <c r="E45" s="11">
-        <v>31.33</v>
-      </c>
-      <c r="F45" s="11">
-        <v>55.34</v>
-      </c>
-      <c r="G45" s="11">
-        <v>7395.23</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I45" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
     </row>
     <row r="46" spans="1:11" ht="16.5">
-      <c r="A46" s="11">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="C46" s="11">
-        <v>112.96</v>
-      </c>
-      <c r="D46" s="11">
-        <v>47.8</v>
-      </c>
-      <c r="E46" s="11">
-        <v>37.04</v>
-      </c>
-      <c r="F46" s="11">
-        <v>55.44</v>
-      </c>
-      <c r="G46" s="11">
-        <v>18421.419999999998</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
     <row r="47" spans="1:11" ht="16.5">
-      <c r="A47" s="11">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="11">
-        <v>2.96</v>
-      </c>
-      <c r="C47" s="11">
-        <v>87.82</v>
-      </c>
-      <c r="D47" s="11">
-        <v>44.8</v>
-      </c>
-      <c r="E47" s="11">
-        <v>5.69</v>
-      </c>
-      <c r="F47" s="11">
-        <v>54.21</v>
-      </c>
-      <c r="G47" s="11">
-        <v>2595.65</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I47" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
     <row r="48" spans="1:11" ht="16.5">
-      <c r="A48" s="11">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" s="11">
-        <v>2.96</v>
-      </c>
-      <c r="C48" s="11">
-        <v>167.32</v>
-      </c>
-      <c r="D48" s="11">
-        <v>46.5</v>
-      </c>
-      <c r="E48" s="11">
-        <v>5.56</v>
-      </c>
-      <c r="F48" s="11">
-        <v>53.95</v>
-      </c>
-      <c r="G48" s="11">
-        <v>2615.27</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
     <row r="49" spans="1:11" ht="16.5">
-      <c r="A49" s="11">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B49" s="11">
-        <v>2.95</v>
-      </c>
-      <c r="C49" s="11">
-        <v>113.31</v>
-      </c>
-      <c r="D49" s="11">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E49" s="11">
-        <v>22.81</v>
-      </c>
-      <c r="F49" s="11">
-        <v>48.79</v>
-      </c>
-      <c r="G49" s="11">
-        <v>1733.17</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
     </row>
     <row r="50" spans="1:11" ht="16.5">
-      <c r="A50" s="11">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B50" s="11">
-        <v>2.94</v>
-      </c>
-      <c r="C50" s="11">
-        <v>112.96</v>
-      </c>
-      <c r="D50" s="11">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="E50" s="11">
-        <v>35.56</v>
-      </c>
-      <c r="F50" s="11">
-        <v>54.98</v>
-      </c>
-      <c r="G50" s="11">
-        <v>7204.65</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
     </row>
     <row r="51" spans="1:11" ht="16.5">
-      <c r="A51" s="11">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B51" s="11">
-        <v>2.94</v>
-      </c>
-      <c r="C51" s="11">
-        <v>143.01</v>
-      </c>
-      <c r="D51" s="11">
-        <v>25.5</v>
-      </c>
-      <c r="E51" s="11">
-        <v>34.49</v>
-      </c>
-      <c r="F51" s="11">
-        <v>55.4</v>
-      </c>
-      <c r="G51" s="11">
-        <v>9129.77</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I51" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
     </row>
     <row r="52" spans="1:11" ht="16.5">
-      <c r="A52" s="11">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B52" s="11">
-        <v>2.94</v>
-      </c>
-      <c r="C52" s="11">
-        <v>157.88999999999999</v>
-      </c>
-      <c r="D52" s="11">
-        <v>22.9</v>
-      </c>
-      <c r="E52" s="11">
-        <v>30.18</v>
-      </c>
-      <c r="F52" s="11">
-        <v>55.46</v>
-      </c>
-      <c r="G52" s="11">
-        <v>7196.6</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I52" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
     </row>
     <row r="53" spans="1:11" ht="16.5">
-      <c r="A53" s="11">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B53" s="11">
-        <v>1.75</v>
-      </c>
-      <c r="C53" s="11">
-        <v>143.01</v>
-      </c>
-      <c r="D53" s="11">
-        <v>125.1</v>
-      </c>
-      <c r="E53" s="11">
-        <v>15</v>
-      </c>
-      <c r="F53" s="11">
-        <v>52.81</v>
-      </c>
-      <c r="G53" s="11">
-        <v>18585.169999999998</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I53" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
       <c r="J53" s="11"/>
       <c r="K53" s="11"/>
     </row>
     <row r="54" spans="1:11" ht="16.5">
-      <c r="A54" s="11">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B54" s="11">
-        <v>1.75</v>
-      </c>
-      <c r="C54" s="11">
-        <v>87.82</v>
-      </c>
-      <c r="D54" s="11">
-        <v>139.1</v>
-      </c>
-      <c r="E54" s="11">
-        <v>9.0299999999999994</v>
-      </c>
-      <c r="F54" s="11">
-        <v>52.61</v>
-      </c>
-      <c r="G54" s="11">
-        <v>12406.55</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I54" s="11" t="s">
-        <v>70</v>
-      </c>
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
     </row>
     <row r="55" spans="1:11" ht="16.5">
-      <c r="A55" s="11">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B55" s="11">
-        <v>1.75</v>
-      </c>
-      <c r="C55" s="11">
-        <v>112.55</v>
-      </c>
-      <c r="D55" s="11">
-        <v>99.5</v>
-      </c>
-      <c r="E55" s="11">
-        <v>14.32</v>
-      </c>
-      <c r="F55" s="11">
-        <v>53.92</v>
-      </c>
-      <c r="G55" s="11">
-        <v>14415.05</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I55" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="J55" s="11"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
       <c r="K55" s="11"/>
     </row>
-    <row r="56" spans="1:11" ht="16.5">
+    <row r="56" spans="1:11">
       <c r="A56" s="5"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -5036,7 +4060,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="11"/>
+      <c r="K56" s="6"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="5"/>
@@ -5117,37 +4141,24 @@
       <c r="K62" s="6"/>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="5"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
       <c r="K63" s="6"/>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="7"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="6"/>
-    </row>
-    <row r="65" spans="11:11">
-      <c r="K65" s="9"/>
+      <c r="K64" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L29:V29"/>
+    <mergeCell ref="L28:V28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5155,11 +4166,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B24"/>
+      <selection activeCell="B10" sqref="B10:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5850,7 +4861,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
@@ -6369,7 +5380,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6417,6 +5428,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100155B07917A39914F9664B9093559A33D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbeff89c08116489e82681c46e7ae15d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f6191221-55a2-427d-afce-6bfcc029a585" xmlns:ns4="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a905948312a67a3512ded1d64743b24d" ns3:_="" ns4:_="">
     <xsd:import namespace="f6191221-55a2-427d-afce-6bfcc029a585"/>
@@ -6633,15 +5653,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6649,6 +5660,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCEF473A-5319-4ED2-888F-44217AC86176}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6663,14 +5682,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>